<commit_message>
renaming all excels, recalc with the 2022_12_Memorial event
</commit_message>
<xml_diff>
--- a/zavodnici_TBD.xlsx
+++ b/zavodnici_TBD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C4D4E4-E47B-4197-9424-FD17EE93EE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E316A607-5853-4ABA-A59D-B852BCD4A726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9996" yWindow="-15168" windowWidth="18372" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="-14820" windowWidth="19668" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pythoned" sheetId="1" r:id="rId1"/>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>